<commit_message>
Add the HTML files
</commit_message>
<xml_diff>
--- a/MenuInterativo.xlsx
+++ b/MenuInterativo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
   <si>
     <t>Termos e Abreviaturas</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>"&gt;</t>
+  </si>
+  <si>
+    <t>Designer Partner</t>
   </si>
 </sst>
 </file>
@@ -623,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,25 +672,26 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
+        <v>29</v>
+      </c>
+      <c r="B2" t="str">
+        <f>A2</f>
+        <v>Designer Partner</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D14" si="0">B2</f>
-        <v>Hardwares</v>
+        <f t="shared" ref="D2" si="0">B2</f>
+        <v>Designer Partner</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H14" si="1">A2</f>
-        <v>Hardwares</v>
+        <f t="shared" ref="H2" si="1">A2</f>
+        <v>Designer Partner</v>
       </c>
       <c r="I2" t="s">
         <v>26</v>
@@ -695,24 +699,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" si="0"/>
-        <v>Instalando programas automaticamente!</v>
+        <f t="shared" ref="D3:D15" si="2">B3</f>
+        <v>Hardwares</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="G3" s="3"/>
       <c r="H3" t="str">
-        <f t="shared" si="1"/>
-        <v>Instalando programas automaticamente!</v>
+        <f t="shared" ref="H3:H15" si="3">A3</f>
+        <v>Hardwares</v>
       </c>
       <c r="I3" t="s">
         <v>26</v>
@@ -720,24 +725,24 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>InteligenciaArtificialPC</v>
+        <f t="shared" si="2"/>
+        <v>Instalando programas automaticamente!</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="1"/>
-        <v>Inteligência Artificial - PC</v>
+        <f t="shared" si="3"/>
+        <v>Instalando programas automaticamente!</v>
       </c>
       <c r="I4" t="s">
         <v>26</v>
@@ -745,24 +750,24 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>InteligenciaArtificialZap</v>
+        <f t="shared" si="2"/>
+        <v>InteligenciaArtificialPC</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="1"/>
-        <v>Inteligência Artificial - Zap</v>
+        <f t="shared" si="3"/>
+        <v>Inteligência Artificial - PC</v>
       </c>
       <c r="I5" t="s">
         <v>26</v>
@@ -770,24 +775,24 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>Malwares</v>
+        <f t="shared" si="2"/>
+        <v>InteligenciaArtificialZap</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="1"/>
-        <v>Malwares</v>
+        <f t="shared" si="3"/>
+        <v>Inteligência Artificial - Zap</v>
       </c>
       <c r="I6" t="s">
         <v>26</v>
@@ -795,24 +800,24 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>Mensageria</v>
+        <f t="shared" si="2"/>
+        <v>Malwares</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="1"/>
-        <v>Mensageria</v>
+        <f t="shared" si="3"/>
+        <v>Malwares</v>
       </c>
       <c r="I7" t="s">
         <v>26</v>
@@ -820,24 +825,24 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>NovidadesEmTI</v>
+        <f t="shared" si="2"/>
+        <v>Mensageria</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="1"/>
-        <v>Novidades em TI</v>
+        <f t="shared" si="3"/>
+        <v>Mensageria</v>
       </c>
       <c r="I8" t="s">
         <v>26</v>
@@ -845,24 +850,24 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>ProtocolosEOutros</v>
+        <f t="shared" si="2"/>
+        <v>NovidadesEmTI</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="1"/>
-        <v>Protocolos &amp; Outros</v>
+        <f t="shared" si="3"/>
+        <v>Novidades em TI</v>
       </c>
       <c r="I9" t="s">
         <v>26</v>
@@ -870,24 +875,24 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>Redes</v>
+        <f t="shared" si="2"/>
+        <v>ProtocolosEOutros</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="1"/>
-        <v>Redes</v>
+        <f t="shared" si="3"/>
+        <v>Protocolos &amp; Outros</v>
       </c>
       <c r="I10" t="s">
         <v>26</v>
@@ -895,24 +900,24 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>SistemaDeAutenticacao</v>
+        <f t="shared" si="2"/>
+        <v>Redes</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="1"/>
-        <v>Sistema de Autenticação</v>
+        <f t="shared" si="3"/>
+        <v>Redes</v>
       </c>
       <c r="I11" t="s">
         <v>26</v>
@@ -920,24 +925,24 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>SistemaDeComunicacao</v>
+        <f t="shared" si="2"/>
+        <v>SistemaDeAutenticacao</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="1"/>
-        <v>Sistema de Comunicação</v>
+        <f t="shared" si="3"/>
+        <v>Sistema de Autenticação</v>
       </c>
       <c r="I12" t="s">
         <v>26</v>
@@ -945,24 +950,24 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>SitesDeNoticiasSobreTI</v>
+        <f t="shared" si="2"/>
+        <v>SistemaDeComunicacao</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="1"/>
-        <v>Sites de notícias sobre TI</v>
+        <f t="shared" si="3"/>
+        <v>Sistema de Comunicação</v>
       </c>
       <c r="I13" t="s">
         <v>26</v>
@@ -970,49 +975,62 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>SitesDeNoticiasSobreTI</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>Sites de notícias sobre TI</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
         <v>TermosEAbreviaturas</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="1"/>
+      <c r="F15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="3"/>
         <v>Termos e Abreviaturas</v>
       </c>
-      <c r="I14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="str">
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="str">
         <f>D1</f>
         <v>CienciaDeDados</v>
       </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" ref="D17:D31" si="2">D2</f>
-        <v>Hardwares</v>
-      </c>
       <c r="E17" t="s">
         <v>28</v>
       </c>
@@ -1022,8 +1040,8 @@
         <v>27</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="2"/>
-        <v>Instalando programas automaticamente!</v>
+        <f t="shared" ref="D18:D30" si="4">D3</f>
+        <v>Hardwares</v>
       </c>
       <c r="E18" t="s">
         <v>28</v>
@@ -1034,8 +1052,8 @@
         <v>27</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="2"/>
-        <v>InteligenciaArtificialPC</v>
+        <f t="shared" si="4"/>
+        <v>Instalando programas automaticamente!</v>
       </c>
       <c r="E19" t="s">
         <v>28</v>
@@ -1046,8 +1064,8 @@
         <v>27</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="2"/>
-        <v>InteligenciaArtificialZap</v>
+        <f t="shared" si="4"/>
+        <v>InteligenciaArtificialPC</v>
       </c>
       <c r="E20" t="s">
         <v>28</v>
@@ -1058,8 +1076,8 @@
         <v>27</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="2"/>
-        <v>Malwares</v>
+        <f t="shared" si="4"/>
+        <v>InteligenciaArtificialZap</v>
       </c>
       <c r="E21" t="s">
         <v>28</v>
@@ -1070,8 +1088,8 @@
         <v>27</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="2"/>
-        <v>Mensageria</v>
+        <f t="shared" si="4"/>
+        <v>Malwares</v>
       </c>
       <c r="E22" t="s">
         <v>28</v>
@@ -1082,8 +1100,8 @@
         <v>27</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="2"/>
-        <v>NovidadesEmTI</v>
+        <f t="shared" si="4"/>
+        <v>Mensageria</v>
       </c>
       <c r="E23" t="s">
         <v>28</v>
@@ -1094,8 +1112,8 @@
         <v>27</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="2"/>
-        <v>ProtocolosEOutros</v>
+        <f t="shared" si="4"/>
+        <v>NovidadesEmTI</v>
       </c>
       <c r="E24" t="s">
         <v>28</v>
@@ -1106,8 +1124,8 @@
         <v>27</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="2"/>
-        <v>Redes</v>
+        <f t="shared" si="4"/>
+        <v>ProtocolosEOutros</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
@@ -1118,8 +1136,8 @@
         <v>27</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="2"/>
-        <v>SistemaDeAutenticacao</v>
+        <f t="shared" si="4"/>
+        <v>Redes</v>
       </c>
       <c r="E26" t="s">
         <v>28</v>
@@ -1130,8 +1148,8 @@
         <v>27</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="2"/>
-        <v>SistemaDeComunicacao</v>
+        <f t="shared" si="4"/>
+        <v>SistemaDeAutenticacao</v>
       </c>
       <c r="E27" t="s">
         <v>28</v>
@@ -1142,8 +1160,8 @@
         <v>27</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="2"/>
-        <v>SitesDeNoticiasSobreTI</v>
+        <f t="shared" si="4"/>
+        <v>SistemaDeComunicacao</v>
       </c>
       <c r="E28" t="s">
         <v>28</v>
@@ -1154,10 +1172,22 @@
         <v>27</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>SitesDeNoticiasSobreTI</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="4"/>
         <v>TermosEAbreviaturas</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>